<commit_message>
Added send mail feature for failed test cases.
</commit_message>
<xml_diff>
--- a/input/TestCases.xlsx
+++ b/input/TestCases.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
   <si>
     <t>TEST METHOD NAME</t>
   </si>
@@ -71,9 +71,6 @@
   </si>
   <si>
     <t>abc@gmail.com,123456,Enter valid password|abcdef,123456,Enter valid user name or emailid|narendra,Asdf@1234,http://hreck.techeasesystems.in/#/pending-grn</t>
-  </si>
-  <si>
-    <t>No</t>
   </si>
   <si>
     <t>goToCostCentre</t>
@@ -1322,7 +1319,7 @@
   <dimension ref="A1:IV15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1354,7 +1351,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>15</v>
@@ -1369,7 +1366,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4" t="s">
@@ -1382,7 +1379,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4" t="s">
@@ -1395,7 +1392,7 @@
         <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>12</v>
@@ -1410,7 +1407,7 @@
         <v>13</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>14</v>
@@ -1425,7 +1422,7 @@
         <v>9</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>10</v>
@@ -1437,7 +1434,7 @@
     </row>
     <row r="8" spans="1:5" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
test class and excel updated.
</commit_message>
<xml_diff>
--- a/input/TestCases.xlsx
+++ b/input/TestCases.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="38">
   <si>
     <t>TEST METHOD NAME</t>
   </si>
@@ -134,6 +134,9 @@
   </si>
   <si>
     <t>abcdefgh@gmail.com,Please enter valid Email Id|upavptechease@gmail.com,New password is generated and email is sent to registered email address.</t>
+  </si>
+  <si>
+    <t>Test</t>
   </si>
 </sst>
 </file>
@@ -1379,7 +1382,7 @@
   <dimension ref="A1:XFD26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1411,7 +1414,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>15</v>
@@ -1426,7 +1429,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4" t="s">
@@ -1439,7 +1442,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4" t="s">
@@ -1452,7 +1455,7 @@
         <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>12</v>
@@ -1467,7 +1470,7 @@
         <v>13</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>14</v>
@@ -1482,7 +1485,7 @@
         <v>9</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>10</v>
@@ -1510,7 +1513,7 @@
         <v>17</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>36</v>
@@ -17797,8 +17800,12 @@
       <c r="E19" s="4"/>
     </row>
     <row r="20" spans="1:16384" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
+      <c r="A20" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="C20" s="2"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>

</xml_diff>

<commit_message>
added only pass case
</commit_message>
<xml_diff>
--- a/input/TestCases.xlsx
+++ b/input/TestCases.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="38">
   <si>
     <t>TEST METHOD NAME</t>
   </si>
@@ -136,7 +136,7 @@
     <t>abcdefgh@gmail.com,Please enter valid Email Id|upavptechease@gmail.com,New password is generated and email is sent to registered email address.</t>
   </si>
   <si>
-    <t>Test</t>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -1382,7 +1382,7 @@
   <dimension ref="A1:XFD26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -17807,7 +17807,9 @@
         <v>3</v>
       </c>
       <c r="C20" s="2"/>
-      <c r="D20" s="4"/>
+      <c r="D20" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="E20" s="4"/>
     </row>
     <row r="21" spans="1:16384" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>